<commit_message>
update lookup product method to have a higher cc
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AE0104-F29F-451B-9EA5-1574A9E0D1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B3E2C0-67A4-4162-AD5B-43E02B80D0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -474,11 +474,10 @@
     <t>Iacob Andrei</t>
   </si>
   <si>
-    <t>1. Cautarea unei piese dupa nume</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> F02a. Cautarea unei piese dupa nume.
-F02b. Cautarea unui produs dupa nume.</t>
+    <t>1. Cautarea unui produs dupa nume</t>
+  </si>
+  <si>
+    <t>F02b. Cautarea unui produs dupa nume.</t>
   </si>
 </sst>
 </file>
@@ -1250,6 +1249,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1262,51 +1264,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1319,20 +1336,68 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1355,12 +1420,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1376,9 +1435,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1386,73 +1442,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1917,7 +1916,7 @@
   <dimension ref="B1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,12 +1927,12 @@
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B1" s="12"/>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" s="40" t="s">
@@ -2024,8 +2023,8 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="108" t="s">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="41" t="s">
         <v>91</v>
       </c>
       <c r="C11" s="1"/>
@@ -2059,7 +2058,7 @@
   </sheetPr>
   <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -2071,73 +2070,73 @@
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B1" s="12"/>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="49"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="48"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="44"/>
       <c r="F6" s="33"/>
       <c r="G6" s="33"/>
-      <c r="I6" s="41" t="s">
+      <c r="I6" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="Q6" s="41" t="s">
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="Q6" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
+      <c r="R6" s="43"/>
+      <c r="S6" s="43"/>
+      <c r="T6" s="43"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
       <c r="I8" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="Q8" s="46" t="s">
+      <c r="Q8" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="46"/>
-      <c r="S8" s="46"/>
+      <c r="R8" s="59"/>
+      <c r="S8" s="59"/>
       <c r="T8" s="36" t="s">
         <v>1</v>
       </c>
@@ -2146,19 +2145,19 @@
       <c r="B9" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
+      <c r="C9" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
       <c r="F9" s="38"/>
       <c r="G9" s="38"/>
       <c r="I9" s="39"/>
-      <c r="Q9" s="46" t="s">
+      <c r="Q9" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
+      <c r="R9" s="59"/>
+      <c r="S9" s="59"/>
       <c r="T9" s="36" t="s">
         <v>1</v>
       </c>
@@ -2167,11 +2166,11 @@
       <c r="B10" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
+      <c r="C10" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
       <c r="F10" s="38"/>
       <c r="G10" s="38"/>
       <c r="I10" s="50" t="s">
@@ -2183,13 +2182,13 @@
       <c r="M10" s="51"/>
       <c r="N10" s="51"/>
       <c r="O10" s="52"/>
-      <c r="Q10" s="46" t="s">
+      <c r="Q10" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="R10" s="46" t="s">
+      <c r="R10" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="46"/>
+      <c r="S10" s="59"/>
       <c r="T10" s="36" t="s">
         <v>1</v>
       </c>
@@ -2198,11 +2197,11 @@
       <c r="B11" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
+      <c r="C11" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
       <c r="I11" s="53"/>
@@ -2217,11 +2216,11 @@
       <c r="B12" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
+      <c r="C12" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
       <c r="F12" s="38"/>
       <c r="G12" s="38"/>
       <c r="I12" s="53"/>
@@ -2236,11 +2235,11 @@
       <c r="B13" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
+      <c r="C13" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
       <c r="I13" s="53"/>
@@ -2250,22 +2249,22 @@
       <c r="M13" s="54"/>
       <c r="N13" s="54"/>
       <c r="O13" s="55"/>
-      <c r="Q13" s="41" t="s">
+      <c r="Q13" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42"/>
-      <c r="T13" s="42"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="43"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
+      <c r="C14" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
       <c r="I14" s="53"/>
@@ -2287,11 +2286,11 @@
       <c r="Q15" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="R15" s="59" t="s">
+      <c r="R15" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="59"/>
-      <c r="T15" s="59"/>
+      <c r="S15" s="60"/>
+      <c r="T15" s="60"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I16" s="53"/>
@@ -2304,11 +2303,11 @@
       <c r="Q16" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="R16" s="44" t="s">
+      <c r="R16" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="S16" s="44"/>
-      <c r="T16" s="44"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
     </row>
     <row r="17" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I17" s="53"/>
@@ -2321,11 +2320,11 @@
       <c r="Q17" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="R17" s="44" t="s">
+      <c r="R17" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="S17" s="44"/>
-      <c r="T17" s="44"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
     </row>
     <row r="18" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I18" s="53"/>
@@ -2338,11 +2337,11 @@
       <c r="Q18" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="R18" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="S18" s="44"/>
-      <c r="T18" s="44"/>
+      <c r="R18" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="S18" s="45"/>
+      <c r="T18" s="45"/>
     </row>
     <row r="19" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I19" s="53"/>
@@ -2355,11 +2354,11 @@
       <c r="Q19" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="R19" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="S19" s="44"/>
-      <c r="T19" s="44"/>
+      <c r="R19" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="S19" s="45"/>
+      <c r="T19" s="45"/>
     </row>
     <row r="20" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I20" s="53"/>
@@ -2372,11 +2371,11 @@
       <c r="Q20" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="R20" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="S20" s="44"/>
-      <c r="T20" s="44"/>
+      <c r="R20" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="S20" s="45"/>
+      <c r="T20" s="45"/>
     </row>
     <row r="21" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I21" s="53"/>
@@ -2389,11 +2388,11 @@
       <c r="Q21" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="R21" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="S21" s="44"/>
-      <c r="T21" s="44"/>
+      <c r="R21" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="S21" s="45"/>
+      <c r="T21" s="45"/>
     </row>
     <row r="22" spans="9:20" x14ac:dyDescent="0.25">
       <c r="I22" s="53"/>
@@ -2424,6 +2423,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="Q9:S9"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="Q13:T13"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="R21:T21"/>
@@ -2440,14 +2447,6 @@
     <mergeCell ref="Q6:T6"/>
     <mergeCell ref="R17:T17"/>
     <mergeCell ref="R19:T19"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="Q9:S9"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="Q13:T13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="R18:T18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2491,173 +2490,173 @@
   <sheetData>
     <row r="1" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B1" s="12"/>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="48"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="11"/>
     </row>
     <row r="6" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="67" t="s">
+      <c r="D6" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="66" t="s">
+      <c r="E6" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="66"/>
-      <c r="R6" s="66"/>
-      <c r="S6" s="66"/>
-      <c r="T6" s="66"/>
-      <c r="U6" s="66"/>
-      <c r="V6" s="66"/>
-      <c r="W6" s="66"/>
-      <c r="X6" s="66"/>
-      <c r="Y6" s="66"/>
-      <c r="Z6" s="66"/>
-      <c r="AA6" s="66"/>
-      <c r="AB6" s="66"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="61"/>
+      <c r="R6" s="61"/>
+      <c r="S6" s="61"/>
+      <c r="T6" s="61"/>
+      <c r="U6" s="61"/>
+      <c r="V6" s="61"/>
+      <c r="W6" s="61"/>
+      <c r="X6" s="61"/>
+      <c r="Y6" s="61"/>
+      <c r="Z6" s="61"/>
+      <c r="AA6" s="61"/>
+      <c r="AB6" s="61"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="63" t="s">
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="62" t="s">
+      <c r="F7" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="64" t="s">
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="64"/>
-      <c r="S7" s="64"/>
-      <c r="T7" s="64"/>
-      <c r="U7" s="64"/>
-      <c r="V7" s="65" t="s">
+      <c r="Q7" s="65"/>
+      <c r="R7" s="65"/>
+      <c r="S7" s="65"/>
+      <c r="T7" s="65"/>
+      <c r="U7" s="65"/>
+      <c r="V7" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="W7" s="65"/>
-      <c r="X7" s="65"/>
-      <c r="Y7" s="65"/>
-      <c r="Z7" s="65"/>
-      <c r="AA7" s="65"/>
-      <c r="AB7" s="65"/>
+      <c r="W7" s="64"/>
+      <c r="X7" s="64"/>
+      <c r="Y7" s="64"/>
+      <c r="Z7" s="64"/>
+      <c r="AA7" s="64"/>
+      <c r="AB7" s="64"/>
     </row>
     <row r="8" spans="2:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="66"/>
-      <c r="C8" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="63"/>
-      <c r="F8" s="62" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="69"/>
+      <c r="F8" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62" t="s">
+      <c r="G8" s="68"/>
+      <c r="H8" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62" t="s">
+      <c r="I8" s="68"/>
+      <c r="J8" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62" t="s">
+      <c r="K8" s="68"/>
+      <c r="L8" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="O8" s="62"/>
-      <c r="P8" s="64" t="s">
+      <c r="O8" s="68"/>
+      <c r="P8" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="Q8" s="64" t="s">
+      <c r="Q8" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="R8" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="S8" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="T8" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="U8" s="64" t="s">
+      <c r="R8" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="V8" s="65">
+      <c r="V8" s="64">
         <v>0</v>
       </c>
-      <c r="W8" s="65">
-        <v>1</v>
-      </c>
-      <c r="X8" s="65">
+      <c r="W8" s="64">
+        <v>1</v>
+      </c>
+      <c r="X8" s="64">
         <v>2</v>
       </c>
-      <c r="Y8" s="65" t="s">
+      <c r="Y8" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="Z8" s="65" t="s">
+      <c r="Z8" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="AA8" s="65" t="s">
+      <c r="AA8" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="AB8" s="65" t="s">
+      <c r="AB8" s="64" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="66"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="63"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="69"/>
       <c r="F9" s="13" t="s">
         <v>27</v>
       </c>
@@ -2688,19 +2687,19 @@
       <c r="O9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="P9" s="64"/>
-      <c r="Q9" s="64"/>
-      <c r="R9" s="64"/>
-      <c r="S9" s="64"/>
-      <c r="T9" s="64"/>
-      <c r="U9" s="64"/>
-      <c r="V9" s="65"/>
-      <c r="W9" s="65"/>
-      <c r="X9" s="65"/>
-      <c r="Y9" s="65"/>
-      <c r="Z9" s="65"/>
-      <c r="AA9" s="65"/>
-      <c r="AB9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="65"/>
+      <c r="S9" s="65"/>
+      <c r="T9" s="65"/>
+      <c r="U9" s="65"/>
+      <c r="V9" s="64"/>
+      <c r="W9" s="64"/>
+      <c r="X9" s="64"/>
+      <c r="Y9" s="64"/>
+      <c r="Z9" s="64"/>
+      <c r="AA9" s="64"/>
+      <c r="AB9" s="64"/>
     </row>
     <row r="10" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
@@ -2903,6 +2902,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:O7"/>
+    <mergeCell ref="P7:U7"/>
+    <mergeCell ref="AB8:AB9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B6:B9"/>
@@ -2919,20 +2932,6 @@
     <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="V7:AB7"/>
-    <mergeCell ref="AB8:AB9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:O7"/>
-    <mergeCell ref="P7:U7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2967,55 +2966,55 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="12"/>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="88" t="s">
+      <c r="E4" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="88" t="s">
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="89"/>
+      <c r="L4" s="74"/>
     </row>
     <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="96"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="102"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="83"/>
       <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
@@ -3028,10 +3027,10 @@
       <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="90" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="91"/>
+      <c r="I5" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="76"/>
       <c r="K5" s="2" t="s">
         <v>4</v>
       </c>
@@ -3043,7 +3042,7 @@
       <c r="B6" s="23">
         <v>9</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="77" t="s">
         <v>47</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -3061,10 +3060,10 @@
       <c r="H6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="86" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="87"/>
+      <c r="I6" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="85"/>
       <c r="K6" s="24" t="s">
         <v>1</v>
       </c>
@@ -3076,7 +3075,7 @@
       <c r="B7" s="23">
         <v>10</v>
       </c>
-      <c r="C7" s="97"/>
+      <c r="C7" s="77"/>
       <c r="D7" s="4" t="s">
         <v>54</v>
       </c>
@@ -3092,10 +3091,10 @@
       <c r="H7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="89"/>
+      <c r="I7" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="74"/>
       <c r="K7" s="23" t="s">
         <v>1</v>
       </c>
@@ -3107,7 +3106,7 @@
       <c r="B8" s="23">
         <v>11</v>
       </c>
-      <c r="C8" s="97"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="10" t="s">
         <v>1</v>
       </c>
@@ -3123,10 +3122,10 @@
       <c r="H8" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="89"/>
+      <c r="I8" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="74"/>
       <c r="K8" s="23" t="s">
         <v>1</v>
       </c>
@@ -3138,7 +3137,7 @@
       <c r="B9" s="23">
         <v>12</v>
       </c>
-      <c r="C9" s="97"/>
+      <c r="C9" s="77"/>
       <c r="D9" s="10" t="s">
         <v>1</v>
       </c>
@@ -3154,10 +3153,10 @@
       <c r="H9" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="89"/>
+      <c r="I9" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="74"/>
       <c r="K9" s="23" t="s">
         <v>1</v>
       </c>
@@ -3169,7 +3168,7 @@
       <c r="B10" s="2">
         <v>13</v>
       </c>
-      <c r="C10" s="98"/>
+      <c r="C10" s="78"/>
       <c r="D10" s="9" t="s">
         <v>1</v>
       </c>
@@ -3185,10 +3184,10 @@
       <c r="H10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="90" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="91"/>
+      <c r="I10" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="76"/>
       <c r="K10" s="2" t="s">
         <v>1</v>
       </c>
@@ -3216,83 +3215,83 @@
       <c r="K12" s="25"/>
     </row>
     <row r="13" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="103" t="s">
+      <c r="B13" s="88" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="104"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="105" t="s">
+      <c r="C13" s="89"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="107" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="106"/>
-      <c r="H13" s="103" t="s">
+      <c r="G13" s="108"/>
+      <c r="H13" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="104"/>
-      <c r="L13" s="107"/>
-      <c r="M13" s="73" t="s">
+      <c r="I13" s="89"/>
+      <c r="J13" s="89"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="90"/>
+      <c r="M13" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="N13" s="74"/>
+      <c r="N13" s="96"/>
     </row>
     <row r="14" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="76" t="s">
+      <c r="C14" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="76" t="s">
+      <c r="D14" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="78" t="s">
+      <c r="E14" s="98" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="80" t="s">
+      <c r="F14" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="82" t="s">
+      <c r="G14" s="102" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="84" t="s">
+      <c r="H14" s="103" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="76" t="s">
+      <c r="I14" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="J14" s="76" t="s">
+      <c r="J14" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="K14" s="92" t="s">
+      <c r="K14" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="L14" s="69" t="s">
+      <c r="L14" s="91" t="s">
         <v>81</v>
       </c>
-      <c r="M14" s="71" t="s">
+      <c r="M14" s="93" t="s">
         <v>82</v>
       </c>
-      <c r="N14" s="83" t="s">
+      <c r="N14" s="80" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="75"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="85"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="93"/>
-      <c r="L15" s="70"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="80"/>
+      <c r="B15" s="97"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="101"/>
+      <c r="G15" s="102"/>
+      <c r="H15" s="104"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="106"/>
+      <c r="L15" s="92"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="100"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="29">
@@ -3334,6 +3333,23 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="M13:N13"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:L3"/>
     <mergeCell ref="B4:B5"/>
@@ -3348,23 +3364,6 @@
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3372,12 +3371,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3525,15 +3521,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3557,10 +3557,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC4FB184-C14D-4C2C-BD91-7F8240B2478B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFB6F214-3FD3-47D7-BFB6-77D735E8F784}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>